<commit_message>
updated db schema(added reference table for paymenttype,CRS), modified excel sheet and import code for CRS code. working payment function
</commit_message>
<xml_diff>
--- a/Files/project_hongkong/AEOI_Report.xlsx
+++ b/Files/project_hongkong/AEOI_Report.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian.m.perez\Desktop\project_hongkong\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adrian.m.perez\Documents\Visual Studio 2015\Projects\Project_XML\Files\project_hongkong\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17670" yWindow="0" windowWidth="23070" windowHeight="9720" tabRatio="915"/>
+    <workbookView xWindow="19530" yWindow="0" windowWidth="23070" windowHeight="9720" tabRatio="915"/>
   </bookViews>
   <sheets>
     <sheet name="Remarks" sheetId="18" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="316">
   <si>
     <t>AeoiId</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>CRS103</t>
-  </si>
-  <si>
-    <t>Passive Non-Financial Entity with one or more controlling person that is a Reportable Person</t>
   </si>
   <si>
     <t>Reportable Person</t>
@@ -1384,6 +1381,24 @@
   </si>
   <si>
     <t>No Controlling Persons for Individual Account Holders</t>
+  </si>
+  <si>
+    <t>Passive NFE with one or more controlling person that is a Reportable Person</t>
+  </si>
+  <si>
+    <t>CRS104</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Not really included in the schema. Just for data representation.</t>
+  </si>
+  <si>
+    <t>Non-Reportable Person</t>
+  </si>
+  <si>
+    <t>Non-reportable(crs status) accounts won't be reported. The client must only include the reportable accounts in the data sheet</t>
   </si>
 </sst>
 </file>
@@ -2054,7 +2069,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2066,10 +2081,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
+        <v>278</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>279</v>
-      </c>
-      <c r="B1" s="41" t="s">
-        <v>280</v>
       </c>
       <c r="C1" s="41" t="s">
         <v>50</v>
@@ -2080,7 +2095,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C2" s="42"/>
     </row>
@@ -2089,7 +2104,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="42" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C3" s="42"/>
     </row>
@@ -2098,7 +2113,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C4" s="42"/>
     </row>
@@ -2107,7 +2122,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C5" s="42"/>
     </row>
@@ -2116,7 +2131,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="42" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C6" s="42"/>
     </row>
@@ -2125,7 +2140,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C7" s="42"/>
     </row>
@@ -2134,7 +2149,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C8" s="42"/>
     </row>
@@ -2143,10 +2158,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="24" x14ac:dyDescent="0.25">
@@ -2154,7 +2169,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C10" s="42"/>
     </row>
@@ -2163,7 +2178,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C11" s="42"/>
     </row>
@@ -2172,47 +2187,49 @@
         <v>11</v>
       </c>
       <c r="B12" s="42" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C12" s="42"/>
     </row>
     <row r="13" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="42" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="84" x14ac:dyDescent="0.25">
       <c r="B14" s="42" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="36" x14ac:dyDescent="0.25">
       <c r="B15" s="43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="24" x14ac:dyDescent="0.25">
       <c r="B16" s="42" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="24" x14ac:dyDescent="0.25">
       <c r="B17" s="42" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="18" spans="2:2" ht="36" x14ac:dyDescent="0.25">
       <c r="B18" s="42" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="42" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" s="42"/>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="36" x14ac:dyDescent="0.25">
+      <c r="B20" s="42" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="42"/>
@@ -2259,42 +2276,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2377,7 @@
     <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="38"/>
       <c r="B4" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
@@ -2371,10 +2388,10 @@
     </row>
     <row r="5" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>196</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -2395,7 +2412,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>35</v>
@@ -2411,7 +2428,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H7" s="19" t="s">
         <v>50</v>
@@ -2422,7 +2439,7 @@
         <v>34</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C8" s="52" t="s">
         <v>18</v>
@@ -2438,7 +2455,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="55"/>
       <c r="B9" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C9" s="52" t="s">
         <v>21</v>
@@ -2485,7 +2502,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>0</v>
@@ -2540,7 +2557,7 @@
         <v>58</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -2574,13 +2591,13 @@
         <v>40</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>59</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2589,7 +2606,7 @@
         <v>5</v>
       </c>
       <c r="C17" s="59" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D17" s="59"/>
       <c r="E17" s="30">
@@ -2622,7 +2639,7 @@
         <v>59</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -2636,7 +2653,7 @@
       <c r="D19" s="53"/>
       <c r="E19" s="30"/>
       <c r="F19" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>59</v>
@@ -2645,7 +2662,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>22</v>
@@ -2662,12 +2679,12 @@
         <v>59</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>24</v>
@@ -2729,7 +2746,7 @@
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H24" s="8"/>
     </row>
@@ -2748,7 +2765,7 @@
         <v>59</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -2771,13 +2788,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="55" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="54" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D27" s="54"/>
       <c r="E27" s="33">
@@ -2804,13 +2821,13 @@
         <v>40</v>
       </c>
       <c r="F28" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>59</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -2826,13 +2843,13 @@
         <v>20</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G29" s="13" t="s">
         <v>58</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2848,13 +2865,13 @@
         <v>40</v>
       </c>
       <c r="F30" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G30" s="13" t="s">
         <v>58</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -2870,24 +2887,24 @@
         <v>72</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>58</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="57" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B32" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="54" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D32" s="54"/>
       <c r="E32" s="30">
@@ -2929,10 +2946,10 @@
       <c r="E34" s="30"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2947,7 +2964,7 @@
       <c r="E35" s="30"/>
       <c r="F35" s="17"/>
       <c r="G35" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H35" s="8"/>
     </row>
@@ -2963,10 +2980,10 @@
       <c r="E36" s="30"/>
       <c r="F36" s="17"/>
       <c r="G36" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2981,7 +2998,7 @@
       <c r="E37" s="30"/>
       <c r="F37" s="17"/>
       <c r="G37" s="37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H37" s="8"/>
     </row>
@@ -3020,7 +3037,7 @@
     <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="57"/>
       <c r="B40" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C40" s="53" t="s">
         <v>12</v>
@@ -3034,15 +3051,15 @@
         <v>59</v>
       </c>
       <c r="H40" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C41" s="52" t="s">
         <v>83</v>
@@ -3053,7 +3070,7 @@
       <c r="E41" s="33"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H41" s="12"/>
     </row>
@@ -3067,7 +3084,7 @@
       <c r="E42" s="33"/>
       <c r="F42" s="13"/>
       <c r="G42" s="52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H42" s="12"/>
     </row>
@@ -3076,7 +3093,7 @@
       <c r="B43" s="52"/>
       <c r="C43" s="52"/>
       <c r="D43" s="39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E43" s="33">
         <v>12</v>
@@ -3089,10 +3106,10 @@
     </row>
     <row r="44" spans="1:9" ht="285" x14ac:dyDescent="0.25">
       <c r="A44" s="57" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" s="53" t="s">
         <v>84</v>
@@ -3104,34 +3121,34 @@
         <v>59</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I44" s="21"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="57"/>
       <c r="B45" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C45" s="54" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D45" s="54"/>
       <c r="E45" s="30">
         <v>12</v>
       </c>
       <c r="F45" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H45" s="8"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="57"/>
       <c r="B46" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C46" s="53" t="s">
         <v>21</v>
@@ -3149,17 +3166,17 @@
         <v>33</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" s="54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D47" s="54"/>
       <c r="E47" s="33">
         <v>3</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>59</v>
@@ -3169,41 +3186,41 @@
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="55"/>
       <c r="B48" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C48" s="52" t="s">
         <v>18</v>
       </c>
       <c r="D48" s="52"/>
       <c r="E48" s="33" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>59</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="57" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B49" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C49" s="54" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D49" s="54"/>
       <c r="E49" s="30">
         <v>12</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>59</v>
@@ -3213,7 +3230,7 @@
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="57"/>
       <c r="B50" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C50" s="53" t="s">
         <v>33</v>
@@ -3228,35 +3245,35 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C51" s="54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D51" s="54"/>
       <c r="E51" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>59</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="55"/>
       <c r="B52" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D52" s="52"/>
       <c r="E52" s="33" t="s">
@@ -3264,19 +3281,19 @@
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="55"/>
       <c r="B53" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D53" s="52"/>
       <c r="E53" s="33" t="s">
@@ -3291,10 +3308,10 @@
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="55"/>
       <c r="B54" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C54" s="52" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D54" s="52"/>
       <c r="E54" s="33" t="s">
@@ -3309,37 +3326,37 @@
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="55"/>
       <c r="B55" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D55" s="52"/>
       <c r="E55" s="33"/>
       <c r="F55" s="13"/>
       <c r="G55" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="57" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C56" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" s="54"/>
       <c r="E56" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G56" s="17" t="s">
         <v>59</v>
@@ -3349,10 +3366,10 @@
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="57"/>
       <c r="B57" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C57" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D57" s="53"/>
       <c r="E57" s="30" t="s">
@@ -3360,17 +3377,17 @@
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H57" s="8"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="57"/>
       <c r="B58" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C58" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D58" s="53"/>
       <c r="E58" s="30" t="s">
@@ -3385,10 +3402,10 @@
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="57"/>
       <c r="B59" s="17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C59" s="53" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D59" s="53"/>
       <c r="E59" s="30" t="s">
@@ -3402,30 +3419,30 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="55" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C60" s="54" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D60" s="54"/>
       <c r="E60" s="33">
         <v>2</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H60" s="12"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="55"/>
       <c r="B61" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="52" t="s">
         <v>21</v>
@@ -3434,14 +3451,14 @@
       <c r="E61" s="33"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H61" s="12"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="55"/>
       <c r="B62" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C62" s="52" t="s">
         <v>12</v>
@@ -3458,10 +3475,10 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="57" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B63" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C63" s="53" t="s">
         <v>12</v>
@@ -3479,27 +3496,27 @@
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="57"/>
       <c r="B64" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C64" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D64" s="53"/>
       <c r="E64" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="17" t="s">
         <v>58</v>
       </c>
       <c r="H64" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="57"/>
       <c r="B65" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C65" s="53" t="s">
         <v>12</v>
@@ -3513,13 +3530,13 @@
         <v>59</v>
       </c>
       <c r="H65" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="57"/>
       <c r="B66" s="17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C66" s="53" t="s">
         <v>12</v>
@@ -3537,7 +3554,7 @@
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="57"/>
       <c r="B67" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C67" s="53" t="s">
         <v>12</v>
@@ -3555,7 +3572,7 @@
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="57"/>
       <c r="B68" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C68" s="53" t="s">
         <v>12</v>
@@ -3573,47 +3590,47 @@
     <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="57"/>
       <c r="B69" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C69" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D69" s="53"/>
       <c r="E69" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="17" t="s">
         <v>58</v>
       </c>
       <c r="H69" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="57"/>
       <c r="B70" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C70" s="53" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D70" s="53"/>
       <c r="E70" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="17" t="s">
         <v>58</v>
       </c>
       <c r="H70" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="57"/>
       <c r="B71" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C71" s="53" t="s">
         <v>12</v>
@@ -3631,17 +3648,17 @@
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="57"/>
       <c r="B72" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C72" s="54" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D72" s="54"/>
       <c r="E72" s="30">
         <v>12</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G72" s="17" t="s">
         <v>58</v>
@@ -3651,7 +3668,7 @@
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="57"/>
       <c r="B73" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C73" s="53" t="s">
         <v>21</v>
@@ -3666,49 +3683,49 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="B74" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C74" s="54" t="s">
         <v>246</v>
-      </c>
-      <c r="B74" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C74" s="54" t="s">
-        <v>247</v>
       </c>
       <c r="D74" s="54"/>
       <c r="E74" s="33">
         <v>2</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G74" s="13" t="s">
         <v>59</v>
       </c>
       <c r="H74" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I74" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="55"/>
       <c r="B75" s="52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C75" s="52" t="s">
         <v>83</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E75" s="33"/>
       <c r="F75" s="13"/>
       <c r="G75" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H75" s="12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I75" s="45"/>
     </row>
@@ -3717,15 +3734,15 @@
       <c r="B76" s="52"/>
       <c r="C76" s="52"/>
       <c r="D76" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E76" s="33"/>
       <c r="F76" s="13"/>
       <c r="G76" s="52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H76" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I76" s="45"/>
     </row>
@@ -3734,30 +3751,30 @@
       <c r="B77" s="52"/>
       <c r="C77" s="52"/>
       <c r="D77" s="13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E77" s="33"/>
       <c r="F77" s="13"/>
       <c r="G77" s="52"/>
       <c r="H77" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I77" s="45"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="55"/>
       <c r="B78" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C78" s="52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D78" s="52"/>
       <c r="E78" s="33">
         <v>12</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>58</v>
@@ -3768,7 +3785,7 @@
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="55"/>
       <c r="B79" s="27" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C79" s="52" t="s">
         <v>21</v>
@@ -3784,10 +3801,10 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="57" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C80" s="53" t="s">
         <v>13</v>
@@ -3795,17 +3812,17 @@
       <c r="D80" s="53"/>
       <c r="E80" s="30"/>
       <c r="F80" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G80" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H80" s="8"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="57"/>
       <c r="B81" s="27" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C81" s="53" t="s">
         <v>21</v>
@@ -3821,7 +3838,7 @@
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="57"/>
       <c r="B82" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C82" s="53" t="s">
         <v>12</v>
@@ -3839,7 +3856,7 @@
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="57"/>
       <c r="B83" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C83" s="53" t="s">
         <v>12</v>
@@ -3857,10 +3874,10 @@
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="57"/>
       <c r="B84" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C84" s="53" t="s">
         <v>201</v>
-      </c>
-      <c r="C84" s="53" t="s">
-        <v>202</v>
       </c>
       <c r="D84" s="53"/>
       <c r="E84" s="30"/>
@@ -3872,31 +3889,31 @@
     </row>
     <row r="85" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B85" s="46" t="s">
+        <v>252</v>
+      </c>
+      <c r="C85" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="C85" s="46" t="s">
-        <v>254</v>
-      </c>
       <c r="D85" s="39" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E85" s="33">
         <v>2</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G85" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H85" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="I85" s="50" t="s">
         <v>258</v>
-      </c>
-      <c r="I85" s="50" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -3904,34 +3921,34 @@
       <c r="B86" s="47"/>
       <c r="C86" s="47"/>
       <c r="D86" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E86" s="33"/>
       <c r="F86" s="29"/>
       <c r="G86" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H86" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I86" s="50"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C87" s="54" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D87" s="54"/>
       <c r="E87" s="31">
         <v>2</v>
       </c>
       <c r="F87" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G87" s="16" t="s">
         <v>58</v>
@@ -3941,7 +3958,7 @@
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="56"/>
       <c r="B88" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C88" s="60" t="s">
         <v>21</v>
@@ -3957,7 +3974,7 @@
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="56"/>
       <c r="B89" s="26" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C89" s="60" t="s">
         <v>12</v>
@@ -3967,19 +3984,19 @@
         <v>30</v>
       </c>
       <c r="F89" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G89" s="16" t="s">
         <v>58</v>
       </c>
       <c r="H89" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A90" s="56"/>
       <c r="B90" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C90" s="60" t="s">
         <v>12</v>
@@ -3993,25 +4010,25 @@
         <v>59</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="55" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C91" s="54" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D91" s="54"/>
       <c r="E91" s="33">
         <v>12</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>58</v>
@@ -4021,7 +4038,7 @@
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="55"/>
       <c r="B92" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C92" s="52" t="s">
         <v>21</v>
@@ -4037,7 +4054,7 @@
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="55"/>
       <c r="B93" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C93" s="52" t="s">
         <v>12</v>
@@ -4054,17 +4071,17 @@
     </row>
     <row r="94" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C94" s="60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D94" s="60"/>
       <c r="E94" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F94" s="16"/>
       <c r="G94" s="16" t="s">
@@ -4074,10 +4091,10 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="55" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C95" s="52" t="s">
         <v>12</v>
@@ -4095,7 +4112,7 @@
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="55"/>
       <c r="B96" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C96" s="52" t="s">
         <v>12</v>
@@ -4113,7 +4130,7 @@
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="55"/>
       <c r="B97" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C97" s="52" t="s">
         <v>12</v>
@@ -4131,7 +4148,7 @@
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="55"/>
       <c r="B98" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C98" s="52" t="s">
         <v>12</v>
@@ -4149,7 +4166,7 @@
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="55"/>
       <c r="B99" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C99" s="52" t="s">
         <v>12</v>
@@ -4167,7 +4184,7 @@
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="55"/>
       <c r="B100" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C100" s="52" t="s">
         <v>12</v>
@@ -4185,7 +4202,7 @@
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="55"/>
       <c r="B101" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C101" s="52" t="s">
         <v>12</v>
@@ -4203,7 +4220,7 @@
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="55"/>
       <c r="B102" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C102" s="52" t="s">
         <v>12</v>
@@ -4221,7 +4238,7 @@
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="55"/>
       <c r="B103" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C103" s="52" t="s">
         <v>12</v>
@@ -5579,48 +5596,63 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="2" max="2" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>86</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C5" t="s">
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -5652,106 +5684,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -5764,7 +5796,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5783,34 +5815,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -5842,58 +5874,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed message type indic code issue (CRS701, CRS702)
</commit_message>
<xml_diff>
--- a/Files/project_hongkong/AEOI_Report.xlsx
+++ b/Files/project_hongkong/AEOI_Report.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19530" yWindow="0" windowWidth="23070" windowHeight="9720" tabRatio="915"/>
+    <workbookView xWindow="21390" yWindow="0" windowWidth="23070" windowHeight="9720" tabRatio="915"/>
   </bookViews>
   <sheets>
     <sheet name="Remarks" sheetId="18" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="319">
   <si>
     <t>AeoiId</t>
   </si>
@@ -1399,6 +1399,15 @@
   </si>
   <si>
     <t>Non-reportable(crs status) accounts won't be reported. The client must only include the reportable accounts in the data sheet</t>
+  </si>
+  <si>
+    <t>Place of brith - incluse city and subcity fields(optional)</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Perform Data file validation (e.g., msgtypeIndiCOde to DocSpecCode, etc.)</t>
   </si>
 </sst>
 </file>
@@ -2069,7 +2078,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,39 +2220,49 @@
         <v>305</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="24" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="24" x14ac:dyDescent="0.25">
       <c r="B17" s="42" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="36" x14ac:dyDescent="0.25">
       <c r="B18" s="42" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="42" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="36" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="36" x14ac:dyDescent="0.25">
       <c r="B20" s="42" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="42"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="42"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="24" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>316</v>
+      </c>
+      <c r="C21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="24" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
+        <v>318</v>
+      </c>
+      <c r="C22" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="42"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="42"/>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="42"/>
     </row>
   </sheetData>

</xml_diff>